<commit_message>
fixed consideration of research
</commit_message>
<xml_diff>
--- a/literature/04.reseach-interface-comparative-experiments/20151001-山中-ゾンビグラフあり.xlsx
+++ b/literature/04.reseach-interface-comparative-experiments/20151001-山中-ゾンビグラフあり.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr date1904="1" showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14580" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="13680" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="20151001-山中-ゾンビグラフあり.ラグランジェ" sheetId="1" r:id="rId1"/>
@@ -818,11 +818,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2110606136"/>
-        <c:axId val="-2110716008"/>
+        <c:axId val="2121996840"/>
+        <c:axId val="-2127879256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2110606136"/>
+        <c:axId val="2121996840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -845,19 +845,20 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2110716008"/>
+        <c:crossAx val="-2127879256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2110716008"/>
+        <c:axId val="-2127879256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -882,25 +883,32 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2110606136"/>
+        <c:crossAx val="2121996840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -1202,11 +1210,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2110589960"/>
-        <c:axId val="-2105721960"/>
+        <c:axId val="-2128754584"/>
+        <c:axId val="-2129179272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2110589960"/>
+        <c:axId val="-2128754584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1229,19 +1237,20 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2105721960"/>
+        <c:crossAx val="-2129179272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2105721960"/>
+        <c:axId val="-2129179272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -1266,19 +1275,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2110589960"/>
+        <c:crossAx val="-2128754584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1559,11 +1570,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2108009208"/>
-        <c:axId val="-2112295640"/>
+        <c:axId val="2118552696"/>
+        <c:axId val="2104349064"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2108009208"/>
+        <c:axId val="2118552696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1592,12 +1603,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2112295640"/>
+        <c:crossAx val="2104349064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2112295640"/>
+        <c:axId val="2104349064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -1627,7 +1638,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2108009208"/>
+        <c:crossAx val="2118552696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1914,11 +1925,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2085196840"/>
-        <c:axId val="-2109032344"/>
+        <c:axId val="-2121509592"/>
+        <c:axId val="-2126721256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2085196840"/>
+        <c:axId val="-2121509592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="7.0"/>
@@ -1949,12 +1960,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2109032344"/>
+        <c:crossAx val="-2126721256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2109032344"/>
+        <c:axId val="-2126721256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1984,7 +1995,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2085196840"/>
+        <c:crossAx val="-2121509592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2466,8 +2477,8 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16:I22"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="13" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -3425,7 +3436,7 @@
   <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>

</xml_diff>